<commit_message>
added test case for empty row in xlsx
</commit_message>
<xml_diff>
--- a/ice/tests/test_data/batch_example.xlsx
+++ b/ice/tests/test_data/batch_example.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Label</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>TCGGAGATCAATCTC</t>
+  </si>
+  <si>
+    <t>missing_filepaths</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,6 +673,14 @@
       </c>
       <c r="F10" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>